<commit_message>
Update Docs and Layout UT inheritance
</commit_message>
<xml_diff>
--- a/ECB2_Lib.Parser.Grammar/Tokens.xlsx
+++ b/ECB2_Lib.Parser.Grammar/Tokens.xlsx
@@ -5,13 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Tokens" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Color Basic" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Extended Color Basic" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Disk Basic" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Super Extended Color Basic" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Disk Basic" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Dragon" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="394">
   <si>
     <t xml:space="preserve">Language</t>
   </si>
@@ -37,9 +39,6 @@
     <t xml:space="preserve">Disk Color BASIC</t>
   </si>
   <si>
-    <t xml:space="preserve">Extended Color BASIC</t>
-  </si>
-  <si>
     <t xml:space="preserve">Extended Color Basic 2</t>
   </si>
   <si>
@@ -533,6 +532,9 @@
   </si>
   <si>
     <t xml:space="preserve">Color Basic 1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CoCo 1</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -920,6 +922,9 @@
     <t xml:space="preserve">Extended Color Basic 1.1</t>
   </si>
   <si>
+    <t xml:space="preserve">CoCo 1 and 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Version 1.0</t>
   </si>
   <si>
@@ -1112,6 +1117,15 @@
     <t xml:space="preserve">TM error if variable is numeric, syntax check for “;”, FC error if no more print items, FC Error if format string is null, !#+.% and much more</t>
   </si>
   <si>
+    <t xml:space="preserve">Extended Color Basic 2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CoCo 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disk Extended Color Basic 2.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Disk Color Basic 1.1</t>
   </si>
   <si>
@@ -1215,6 +1229,21 @@
   </si>
   <si>
     <t xml:space="preserve">Warm start OS9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dragon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOSplus 4.9B 3S 1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16K Interpreter 1.0 by 1982 by MS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microcolor Basic 1.0</t>
   </si>
 </sst>
 </file>
@@ -1324,11 +1353,11 @@
   </sheetPr>
   <dimension ref="A1:G162"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A148" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.85"/>
@@ -1354,178 +1383,175 @@
       <c r="C2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1534,208 +1560,208 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1744,45 +1770,45 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1791,104 +1817,104 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1897,11 +1923,11 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1910,11 +1936,11 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1923,11 +1949,11 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1936,28 +1962,28 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1966,16 +1992,16 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -1983,73 +2009,73 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -2057,88 +2083,88 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -2147,68 +2173,68 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -2217,11 +2243,11 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -2230,11 +2256,11 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -2243,46 +2269,46 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2293,306 +2319,306 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -2601,100 +2627,100 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
@@ -2703,51 +2729,51 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -2756,11 +2782,11 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -2769,24 +2795,24 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -2795,28 +2821,28 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -2825,37 +2851,37 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
@@ -2864,30 +2890,30 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
@@ -2896,32 +2922,32 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
@@ -2930,519 +2956,519 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F110" s="1"/>
       <c r="G110" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F116" s="1"/>
       <c r="G116" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F121" s="1"/>
       <c r="G121" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B124" s="1"/>
       <c r="C124" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B127" s="1"/>
       <c r="C127" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F128" s="1"/>
       <c r="G128" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F129" s="1"/>
       <c r="G129" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B130" s="1"/>
       <c r="C130" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
@@ -3451,133 +3477,133 @@
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F133" s="1"/>
       <c r="G133" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F134" s="1"/>
       <c r="G134" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F135" s="1"/>
       <c r="G135" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F136" s="1"/>
       <c r="G136" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B137" s="1"/>
       <c r="C137" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
@@ -3586,32 +3612,32 @@
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F138" s="1"/>
       <c r="G138" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B139" s="1"/>
       <c r="C139" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
@@ -3620,11 +3646,11 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B140" s="1"/>
       <c r="C140" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
@@ -3633,199 +3659,199 @@
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F141" s="1"/>
       <c r="G141" s="1"/>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F142" s="1"/>
       <c r="G142" s="1"/>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F143" s="1"/>
       <c r="G143" s="1"/>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F144" s="1"/>
       <c r="G144" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F145" s="1"/>
       <c r="G145" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
       <c r="D146" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
       <c r="D147" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F147" s="1"/>
       <c r="G147" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F150" s="1"/>
       <c r="G150" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
@@ -3834,130 +3860,130 @@
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F152" s="1"/>
       <c r="G152" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F154" s="1"/>
       <c r="G154" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F155" s="1"/>
       <c r="G155" s="1"/>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F156" s="1"/>
       <c r="G156" s="1"/>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F157" s="1"/>
       <c r="G157" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F158" s="1"/>
       <c r="G158" s="1"/>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B159" s="1"/>
       <c r="C159" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D159" s="1"/>
       <c r="E159" s="1"/>
@@ -3966,24 +3992,24 @@
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
       <c r="E160" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F160" s="1"/>
       <c r="G160" s="1"/>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B161" s="1"/>
       <c r="C161" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D161" s="1"/>
       <c r="E161" s="1"/>
@@ -3992,10 +4018,10 @@
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G162" s="1"/>
     </row>
@@ -4017,17 +4043,20 @@
   </sheetPr>
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.06"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>169</v>
       </c>
     </row>
@@ -4266,7 +4295,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>128</v>
@@ -4275,7 +4304,7 @@
         <v>216</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H51" s="0" t="n">
         <v>128</v>
@@ -4295,7 +4324,7 @@
         <v>219</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H52" s="0" t="n">
         <v>129</v>
@@ -4306,7 +4335,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>130</v>
@@ -4315,7 +4344,7 @@
         <v>221</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H53" s="0" t="n">
         <v>130</v>
@@ -4332,7 +4361,7 @@
         <v>131</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H54" s="0" t="n">
         <v>131</v>
@@ -4349,7 +4378,7 @@
         <v>225</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H55" s="0" t="n">
         <v>132</v>
@@ -4369,7 +4398,7 @@
         <v>228</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H56" s="0" t="n">
         <v>133</v>
@@ -4377,7 +4406,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>134</v>
@@ -4386,7 +4415,7 @@
         <v>229</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H57" s="0" t="n">
         <v>134</v>
@@ -4394,7 +4423,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>135</v>
@@ -4403,7 +4432,7 @@
         <v>230</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H58" s="0" t="n">
         <v>135</v>
@@ -4423,7 +4452,7 @@
         <v>233</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H59" s="0" t="n">
         <v>136</v>
@@ -4434,7 +4463,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>137</v>
@@ -4443,7 +4472,7 @@
         <v>235</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H60" s="0" t="n">
         <v>137</v>
@@ -4454,7 +4483,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>138</v>
@@ -4463,7 +4492,7 @@
         <v>237</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H61" s="0" t="n">
         <v>138</v>
@@ -4483,7 +4512,7 @@
         <v>240</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H62" s="0" t="n">
         <v>139</v>
@@ -4494,13 +4523,13 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>140</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H63" s="0" t="n">
         <v>140</v>
@@ -4508,7 +4537,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>141</v>
@@ -4517,7 +4546,7 @@
         <v>242</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H64" s="0" t="n">
         <v>141</v>
@@ -4528,7 +4557,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>142</v>
@@ -4537,7 +4566,7 @@
         <v>244</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H65" s="0" t="n">
         <v>142</v>
@@ -4545,13 +4574,13 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>143</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H66" s="0" t="n">
         <v>143</v>
@@ -4559,7 +4588,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>144</v>
@@ -4568,7 +4597,7 @@
         <v>245</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H67" s="0" t="n">
         <v>144</v>
@@ -4579,7 +4608,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>145</v>
@@ -4588,7 +4617,7 @@
         <v>247</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H68" s="0" t="n">
         <v>145</v>
@@ -4599,13 +4628,13 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>146</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H69" s="0" t="n">
         <v>146</v>
@@ -4613,7 +4642,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>147</v>
@@ -4622,7 +4651,7 @@
         <v>249</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H70" s="0" t="n">
         <v>147</v>
@@ -4633,7 +4662,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>148</v>
@@ -4644,7 +4673,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>149</v>
@@ -4655,7 +4684,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>150</v>
@@ -4666,7 +4695,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>151</v>
@@ -4674,7 +4703,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>152</v>
@@ -4682,7 +4711,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>153</v>
@@ -4698,7 +4727,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>155</v>
@@ -4709,7 +4738,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>156</v>
@@ -4720,7 +4749,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>157</v>
@@ -4728,7 +4757,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>158</v>
@@ -4739,7 +4768,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>159</v>
@@ -4747,7 +4776,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>160</v>
@@ -4755,7 +4784,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>161</v>
@@ -4766,7 +4795,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>162</v>
@@ -4774,7 +4803,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>163</v>
@@ -4936,7 +4965,7 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C105" s="0" t="s">
         <v>280</v>
@@ -4984,16 +5013,19 @@
   </sheetPr>
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C60" activeCellId="0" sqref="C60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>285</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -5002,147 +5034,147 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5152,95 +5184,95 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>181</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>148</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>182</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>149</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>183</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>150</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>184</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>151</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>185</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>152</v>
@@ -5248,33 +5280,33 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>186</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>153</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>187</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>154</v>
@@ -5282,30 +5314,30 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>188</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>155</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>189</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>156</v>
@@ -5313,50 +5345,50 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>190</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>157</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>191</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>158</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>192</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>159</v>
@@ -5364,33 +5396,33 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>193</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>160</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>194</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E54" s="0" t="n">
         <v>161</v>
@@ -5398,7 +5430,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>195</v>
@@ -5406,7 +5438,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>196</v>
@@ -5414,7 +5446,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>197</v>
@@ -5422,7 +5454,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>198</v>
@@ -5430,7 +5462,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>199</v>
@@ -5438,7 +5470,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>200</v>
@@ -5446,7 +5478,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>201</v>
@@ -5454,7 +5486,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>202</v>
@@ -5462,18 +5494,18 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>203</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>204</v>
@@ -5481,7 +5513,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>205</v>
@@ -5489,84 +5521,84 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -5585,17 +5617,54 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A9:C10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>353</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5605,27 +5674,27 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5635,61 +5704,61 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>206</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>162</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>207</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>163</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>208</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>164</v>
@@ -5697,16 +5766,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>209</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>165</v>
@@ -5714,36 +5783,36 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>210</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>166</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>211</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>167</v>
@@ -5751,18 +5820,18 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>212</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>213</v>
@@ -5770,18 +5839,18 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>214</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>215</v>
@@ -5789,40 +5858,40 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>216</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>217</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>218</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>219</v>
@@ -5830,83 +5899,133 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>220</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>221</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>222</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>223</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>224</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>225</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update docs and UT layout
</commit_message>
<xml_diff>
--- a/ECB2_Lib.Parser.Grammar/Tokens.xlsx
+++ b/ECB2_Lib.Parser.Grammar/Tokens.xlsx
@@ -5,14 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tokens" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Color Basic" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Extended Color Basic" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Super Extended Color Basic" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Disk Basic" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Disk Basic" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Extended Color Basic" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Super Extended Color Basic" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Dragon" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="394">
   <si>
     <t xml:space="preserve">Language</t>
   </si>
@@ -919,6 +919,117 @@
     <t xml:space="preserve">String concatenation.  Type mismatch if numeric variable.  Check if length &gt; 255.  </t>
   </si>
   <si>
+    <t xml:space="preserve">DEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disk Color Basic 1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File type: 0-BASIC, 1-BASIC data, 2-machine language, 3-text editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASCII flag: 0-binary or crunched BASIC, $FF-ASCII</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISK BASIC 1.0 used 6k of ROM.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISK BASIC 1.1 used 6.5k of ROM with .5k of fixes to 1.0.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dragon Computer disk commands take 8k of ROM and include fixes and more features.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary Tokens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary Tokens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FC Error if &lt;&gt; 5 bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max drive number is 3.  Device Error for over 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only 4 legal drives.  Error if Drive Number &gt; 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIELD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Syntax check for comma.  Syntax check for AS token.  TM error if numeric variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 FCBS max.  Illegal function call if more than 15.  Syntax check for comma.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Filename.  Syntax error if too many characters  Error if file is open.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TM Error if VALTYP is string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Syntax check for comma.  Is Next Char ‘R’ after LOAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TM error if numeric variable.  Syntax check for ‘=’ token.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RENAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Syntax check for TO.  FC error if files on different drives.  Verify new file does not exist.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Filename. Save a crunched file.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WRITE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default to current device if not given.  Check device number validity.  Syntax check for comma.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for ON or OFF token.  Syntax error if not found.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSKINI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DN error if no drive number specified.  Calculate drive number.  Syntax check for comma and evaluate expression.  Max value of skip factor is 16.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BACKUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device Number error if no drive numbers given.  Token for ‘TO’.  Syntax for ‘TO’.  Will use more memory if free memory is available.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Token for ‘TO’.  Syntax error for ‘TO’.  OM error if not at least one full sector of free RAM.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DKSI$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluate string variable 1 and 2.  Syntax check for comma.  TM error if numeric variable.  FC error if drive number &gt; 3.  FC error if track number &gt; 34.  Syntax check for comma.  Evaluate expression(sector number).  FC Error if sector number too big.  Syntax check for comma.  Evaluate Routine address.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get the drive, track, and sector numbers.  TM Error if numeric expression.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warm start OS9</t>
+  </si>
+  <si>
     <t xml:space="preserve">Extended Color Basic 1.1</t>
   </si>
   <si>
@@ -1036,9 +1147,6 @@
     <t xml:space="preserve">E**X</t>
   </si>
   <si>
-    <t xml:space="preserve">DEF</t>
-  </si>
-  <si>
     <t xml:space="preserve">Natural or naperian logarithm</t>
   </si>
   <si>
@@ -1069,9 +1177,6 @@
     <t xml:space="preserve">Syntax check for comma, save new interval, check renumber range is valid, </t>
   </si>
   <si>
-    <t xml:space="preserve">FN</t>
-  </si>
-  <si>
     <t xml:space="preserve">USING</t>
   </si>
   <si>
@@ -1124,111 +1229,6 @@
   </si>
   <si>
     <t xml:space="preserve">Disk Extended Color Basic 2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disk Color Basic 1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File type: 0-BASIC, 1-BASIC data, 2-machine language, 3-text editor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASCII flag: 0-binary or crunched BASIC, $FF-ASCII</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DISK BASIC 1.0 used 6k of ROM.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DISK BASIC 1.1 used 6.5k of ROM with .5k of fixes to 1.0.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dragon Computer disk commands take 8k of ROM and include fixes and more features.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary Tokens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secondary Tokens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FC Error if &lt;&gt; 5 bytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max drive number is 3.  Device Error for over 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Only 4 legal drives.  Error if Drive Number &gt; 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FIELD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Syntax check for comma.  Syntax check for AS token.  TM error if numeric variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 FCBS max.  Illegal function call if more than 15.  Syntax check for comma.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get Filename.  Syntax error if too many characters  Error if file is open.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TM Error if VALTYP is string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Syntax check for comma.  Is Next Char ‘R’ after LOAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TM error if numeric variable.  Syntax check for ‘=’ token.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RENAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Syntax check for TO.  FC error if files on different drives.  Verify new file does not exist.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get Filename. Save a crunched file.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WRITE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default to current device if not given.  Check device number validity.  Syntax check for comma.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check for ON or OFF token.  Syntax error if not found.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DSKINI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DN error if no drive number specified.  Calculate drive number.  Syntax check for comma and evaluate expression.  Max value of skip factor is 16.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BACKUP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Device Number error if no drive numbers given.  Token for ‘TO’.  Syntax for ‘TO’.  Will use more memory if free memory is available.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Token for ‘TO’.  Syntax error for ‘TO’.  OM error if not at least one full sector of free RAM.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DKSI$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evaluate string variable 1 and 2.  Syntax check for comma.  TM error if numeric variable.  FC error if drive number &gt; 3.  FC error if track number &gt; 34.  Syntax check for comma.  Evaluate expression(sector number).  FC Error if sector number too big.  Syntax check for comma.  Evaluate Routine address.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get the drive, track, and sector numbers.  TM Error if numeric expression.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warm start OS9</t>
   </si>
   <si>
     <t xml:space="preserve">Dragon</t>
@@ -1253,7 +1253,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1277,6 +1277,13 @@
     </font>
     <font>
       <strike val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1325,13 +1332,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1353,11 +1368,11 @@
   </sheetPr>
   <dimension ref="A1:G162"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.85"/>
@@ -4041,13 +4056,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I108"/>
+  <dimension ref="A1:K110"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.06"/>
   </cols>
@@ -4151,7 +4166,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="2" t="s">
         <v>188</v>
       </c>
     </row>
@@ -4289,685 +4304,907 @@
       <c r="A50" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="G50" s="0" t="s">
+      <c r="H50" s="0" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="0" t="n">
+      <c r="B51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="0" t="n">
         <v>128</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="D51" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="G51" s="0" t="s">
+      <c r="H51" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="H51" s="0" t="n">
+      <c r="I51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J51" s="0" t="n">
         <v>128</v>
       </c>
-      <c r="I51" s="0" t="s">
+      <c r="K51" s="0" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="B52" s="0" t="n">
+      <c r="B52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="0" t="n">
         <v>129</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="D52" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="G52" s="0" t="s">
+      <c r="H52" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="H52" s="0" t="n">
+      <c r="I52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J52" s="0" t="n">
         <v>129</v>
       </c>
-      <c r="I52" s="0" t="s">
+      <c r="K52" s="0" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B53" s="0" t="n">
+      <c r="B53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="D53" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="G53" s="0" t="s">
+      <c r="H53" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H53" s="0" t="n">
+      <c r="I53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J53" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="I53" s="0" t="s">
+      <c r="K53" s="0" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="B54" s="0" t="n">
+      <c r="B54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="0" t="n">
         <v>131</v>
       </c>
-      <c r="G54" s="0" t="s">
+      <c r="H54" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="H54" s="0" t="n">
+      <c r="I54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J54" s="0" t="n">
         <v>131</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B55" s="0" t="n">
+      <c r="B55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="0" t="n">
         <v>132</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="D55" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="G55" s="0" t="s">
+      <c r="H55" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="H55" s="0" t="n">
+      <c r="I55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J55" s="0" t="n">
         <v>132</v>
       </c>
-      <c r="I55" s="0" t="s">
+      <c r="K55" s="0" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="B56" s="0" t="n">
+      <c r="B56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="0" t="n">
         <v>133</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="D56" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="G56" s="0" t="s">
+      <c r="H56" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="H56" s="0" t="n">
+      <c r="I56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J56" s="0" t="n">
         <v>133</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B57" s="0" t="n">
+      <c r="B57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="0" t="n">
         <v>134</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="D57" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="G57" s="0" t="s">
+      <c r="H57" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="H57" s="0" t="n">
+      <c r="I57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J57" s="0" t="n">
         <v>134</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B58" s="0" t="n">
+      <c r="B58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="0" t="n">
         <v>135</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="D58" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="G58" s="0" t="s">
+      <c r="H58" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H58" s="0" t="n">
+      <c r="I58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J58" s="0" t="n">
         <v>135</v>
       </c>
-      <c r="I58" s="0" t="s">
+      <c r="K58" s="0" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="B59" s="0" t="n">
+      <c r="B59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="0" t="n">
         <v>136</v>
       </c>
-      <c r="C59" s="0" t="s">
+      <c r="D59" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="G59" s="0" t="s">
+      <c r="H59" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="H59" s="0" t="n">
+      <c r="I59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J59" s="0" t="n">
         <v>136</v>
       </c>
-      <c r="I59" s="0" t="s">
+      <c r="K59" s="0" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B60" s="0" t="n">
+      <c r="B60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="0" t="n">
         <v>137</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="D60" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="G60" s="0" t="s">
+      <c r="H60" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="H60" s="0" t="n">
+      <c r="I60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J60" s="0" t="n">
         <v>137</v>
       </c>
-      <c r="I60" s="0" t="s">
+      <c r="K60" s="0" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B61" s="0" t="n">
+      <c r="B61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="0" t="n">
         <v>138</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="D61" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="G61" s="0" t="s">
+      <c r="H61" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H61" s="0" t="n">
+      <c r="I61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J61" s="0" t="n">
         <v>138</v>
       </c>
-      <c r="I61" s="0" t="s">
+      <c r="K61" s="0" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B62" s="0" t="n">
+      <c r="B62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" s="0" t="n">
         <v>139</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="D62" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="G62" s="0" t="s">
+      <c r="H62" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H62" s="0" t="n">
+      <c r="I62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J62" s="0" t="n">
         <v>139</v>
       </c>
-      <c r="I62" s="0" t="s">
+      <c r="K62" s="0" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B63" s="0" t="n">
+      <c r="B63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="0" t="n">
         <v>140</v>
       </c>
-      <c r="G63" s="0" t="s">
+      <c r="H63" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H63" s="0" t="n">
+      <c r="I63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J63" s="0" t="n">
         <v>140</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B64" s="0" t="n">
+      <c r="B64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="0" t="n">
         <v>141</v>
       </c>
-      <c r="C64" s="0" t="s">
+      <c r="D64" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="G64" s="0" t="s">
+      <c r="H64" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="H64" s="0" t="n">
+      <c r="I64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J64" s="0" t="n">
         <v>141</v>
       </c>
-      <c r="I64" s="0" t="s">
+      <c r="K64" s="0" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B65" s="0" t="n">
+      <c r="B65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="0" t="n">
         <v>142</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="D65" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="G65" s="0" t="s">
+      <c r="H65" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H65" s="0" t="n">
+      <c r="I65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J65" s="0" t="n">
         <v>142</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B66" s="0" t="n">
+      <c r="B66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" s="0" t="n">
         <v>143</v>
       </c>
-      <c r="G66" s="0" t="s">
+      <c r="H66" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H66" s="0" t="n">
+      <c r="I66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J66" s="0" t="n">
         <v>143</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B67" s="0" t="n">
+      <c r="B67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" s="0" t="n">
         <v>144</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="D67" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="G67" s="0" t="s">
+      <c r="H67" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="H67" s="0" t="n">
+      <c r="I67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J67" s="0" t="n">
         <v>144</v>
       </c>
-      <c r="I67" s="0" t="s">
+      <c r="K67" s="0" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="A68" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B68" s="0" t="n">
+      <c r="B68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" s="0" t="n">
         <v>145</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="D68" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="G68" s="0" t="s">
+      <c r="H68" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="H68" s="0" t="n">
+      <c r="I68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J68" s="0" t="n">
         <v>145</v>
       </c>
-      <c r="I68" s="0" t="s">
+      <c r="K68" s="0" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="A69" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B69" s="0" t="n">
+      <c r="B69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" s="0" t="n">
         <v>146</v>
       </c>
-      <c r="G69" s="0" t="s">
+      <c r="H69" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="H69" s="0" t="n">
+      <c r="I69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J69" s="0" t="n">
         <v>146</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B70" s="0" t="n">
+      <c r="B70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" s="0" t="n">
         <v>147</v>
       </c>
-      <c r="C70" s="0" t="s">
+      <c r="D70" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="G70" s="0" t="s">
+      <c r="H70" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="H70" s="0" t="n">
+      <c r="I70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J70" s="0" t="n">
         <v>147</v>
       </c>
-      <c r="I70" s="0" t="s">
+      <c r="K70" s="0" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="A71" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B71" s="0" t="n">
+      <c r="B71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" s="0" t="n">
         <v>148</v>
       </c>
-      <c r="C71" s="0" t="s">
+      <c r="D71" s="0" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B72" s="0" t="n">
+      <c r="B72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="0" t="n">
         <v>149</v>
       </c>
-      <c r="C72" s="0" t="s">
+      <c r="D72" s="0" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="A73" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B73" s="0" t="n">
+      <c r="B73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="C73" s="0" t="s">
+      <c r="D73" s="0" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="A74" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B74" s="0" t="n">
+      <c r="B74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" s="0" t="n">
         <v>151</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="A75" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B75" s="0" t="n">
+      <c r="B75" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" s="0" t="n">
         <v>152</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+      <c r="A76" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B76" s="0" t="n">
+      <c r="B76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" s="0" t="n">
         <v>153</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="A77" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B77" s="0" t="n">
+      <c r="B77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" s="0" t="n">
         <v>154</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="A78" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B78" s="0" t="n">
+      <c r="B78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" s="0" t="n">
         <v>155</v>
       </c>
-      <c r="C78" s="0" t="s">
+      <c r="D78" s="0" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="A79" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B79" s="0" t="n">
+      <c r="B79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" s="0" t="n">
         <v>156</v>
       </c>
-      <c r="C79" s="0" t="s">
+      <c r="D79" s="0" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+      <c r="A80" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B80" s="0" t="n">
+      <c r="B80" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" s="0" t="n">
         <v>157</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+      <c r="A81" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B81" s="0" t="n">
+      <c r="B81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" s="0" t="n">
         <v>158</v>
       </c>
-      <c r="C81" s="0" t="s">
+      <c r="D81" s="0" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="A82" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B82" s="0" t="n">
+      <c r="B82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" s="0" t="n">
         <v>159</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+      <c r="A83" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B83" s="0" t="n">
+      <c r="B83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" s="0" t="n">
         <v>160</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+      <c r="A84" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B84" s="0" t="n">
+      <c r="B84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" s="0" t="n">
         <v>161</v>
       </c>
-      <c r="C84" s="0" t="s">
+      <c r="D84" s="0" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="A85" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B85" s="0" t="n">
+      <c r="B85" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85" s="0" t="n">
         <v>162</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+      <c r="A86" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B86" s="0" t="n">
+      <c r="B86" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" s="0" t="n">
         <v>163</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+      <c r="A87" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="B87" s="0" t="n">
+      <c r="B87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" s="0" t="n">
         <v>164</v>
       </c>
-      <c r="C87" s="0" t="s">
+      <c r="D87" s="0" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+      <c r="A88" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="B88" s="0" t="n">
+      <c r="B88" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" s="0" t="n">
         <v>165</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+      <c r="A89" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B89" s="0" t="n">
+      <c r="B89" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" s="0" t="n">
         <v>166</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
+      <c r="A90" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="B90" s="0" t="n">
+      <c r="B90" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" s="0" t="n">
         <v>167</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+      <c r="A91" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B91" s="0" t="n">
+      <c r="B91" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" s="0" t="n">
         <v>168</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
+      <c r="A92" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="B92" s="0" t="n">
+      <c r="B92" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" s="0" t="n">
         <v>169</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
+      <c r="A93" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="B93" s="0" t="n">
+      <c r="B93" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C93" s="0" t="n">
         <v>170</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
+      <c r="A94" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B94" s="0" t="n">
+      <c r="B94" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" s="0" t="n">
         <v>171</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
+      <c r="A95" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="B95" s="0" t="n">
+      <c r="B95" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" s="0" t="n">
         <v>172</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
+      <c r="A96" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="B96" s="0" t="n">
+      <c r="B96" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" s="0" t="n">
         <v>173</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
+      <c r="A97" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="B97" s="0" t="n">
+      <c r="B97" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97" s="0" t="n">
         <v>174</v>
       </c>
-      <c r="C97" s="0" t="s">
+      <c r="D97" s="0" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
+      <c r="A98" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B98" s="0" t="n">
+      <c r="B98" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C98" s="0" t="n">
         <v>175</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+      <c r="A99" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="B99" s="0" t="n">
+      <c r="B99" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C99" s="0" t="n">
         <v>176</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
+      <c r="A100" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="B100" s="0" t="n">
+      <c r="B100" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C100" s="0" t="n">
         <v>177</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
+      <c r="A101" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="B101" s="0" t="n">
+      <c r="B101" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C101" s="0" t="n">
         <v>178</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
+      <c r="A102" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="B102" s="0" t="n">
+      <c r="B102" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" s="0" t="n">
         <v>179</v>
       </c>
-      <c r="C102" s="0" t="n">
+      <c r="D102" s="0" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getHex2Dec("80")</f>
         <v>128</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
+      <c r="A103" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="B103" s="0" t="n">
+      <c r="B103" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C103" s="0" t="n">
         <v>180</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
+      <c r="A104" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C104" s="0" t="s">
+      <c r="B104" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D104" s="0" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
+      <c r="A105" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C105" s="0" t="s">
+      <c r="D105" s="0" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4975,12 +5212,12 @@
       <c r="A106" s="0" t="s">
         <v>281</v>
       </c>
-      <c r="C106" s="0" t="s">
+      <c r="D106" s="0" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C107" s="0" t="s">
+      <c r="D107" s="0" t="s">
         <v>283</v>
       </c>
     </row>
@@ -4988,11 +5225,21 @@
       <c r="A108" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="B108" s="0" t="n">
+      <c r="C108" s="0" t="n">
         <v>171</v>
       </c>
-      <c r="C108" s="0" t="s">
+      <c r="D108" s="0" t="s">
         <v>284</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -5011,20 +5258,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5034,571 +5278,308 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+      <c r="D12" s="0" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>206</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>162</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>207</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+      <c r="D14" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>163</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+      <c r="A15" s="0" t="s">
         <v>298</v>
       </c>
+      <c r="B15" s="0" t="n">
+        <v>208</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>164</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
-        <v>299</v>
+      <c r="A16" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>209</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>165</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
-        <v>300</v>
+      <c r="A17" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>166</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
-        <v>301</v>
+      <c r="A18" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>211</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>167</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="s">
-        <v>302</v>
+      <c r="A19" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>212</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
-        <v>303</v>
+      <c r="A20" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>213</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
-        <v>304</v>
+      <c r="A21" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>214</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
-        <v>305</v>
+      <c r="A22" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>215</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
-        <v>306</v>
+      <c r="A23" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>216</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
-        <v>307</v>
+      <c r="A24" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>217</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
-        <v>308</v>
+      <c r="A25" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>218</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
-        <v>309</v>
+      <c r="A26" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>219</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
-        <v>310</v>
+      <c r="A27" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
-        <v>311</v>
+      <c r="A28" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>221</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
-        <v>312</v>
+      <c r="A29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
-        <v>313</v>
+      <c r="A30" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>223</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
-        <v>314</v>
+      <c r="A31" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>224</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
-        <v>315</v>
+      <c r="A32" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>225</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B41" s="0" t="n">
-        <v>181</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41" s="0" t="n">
-        <v>148</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" s="0" t="n">
-        <v>182</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="E42" s="0" t="n">
-        <v>149</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="B43" s="0" t="n">
-        <v>183</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="E43" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B44" s="0" t="n">
-        <v>184</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="E44" s="0" t="n">
-        <v>151</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="B45" s="0" t="n">
-        <v>185</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E45" s="0" t="n">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="B46" s="0" t="n">
-        <v>186</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="E46" s="0" t="n">
-        <v>153</v>
-      </c>
-      <c r="F46" s="0" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B47" s="0" t="n">
-        <v>187</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="E47" s="0" t="n">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="B48" s="0" t="n">
-        <v>188</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="E48" s="0" t="n">
-        <v>155</v>
-      </c>
-      <c r="F48" s="0" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="B49" s="0" t="n">
-        <v>189</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E49" s="0" t="n">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="B50" s="0" t="n">
-        <v>190</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E50" s="0" t="n">
-        <v>157</v>
-      </c>
-      <c r="F50" s="0" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B51" s="0" t="n">
-        <v>191</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="E51" s="0" t="n">
-        <v>158</v>
-      </c>
-      <c r="F51" s="0" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="B52" s="0" t="n">
-        <v>192</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="E52" s="0" t="n">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B53" s="0" t="n">
-        <v>193</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>331</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="E53" s="0" t="n">
-        <v>160</v>
-      </c>
-      <c r="F53" s="0" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B54" s="0" t="n">
-        <v>194</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="E54" s="0" t="n">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="B55" s="0" t="n">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B56" s="0" t="n">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="B57" s="0" t="n">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B58" s="0" t="n">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="B59" s="0" t="n">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="B60" s="0" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="B61" s="0" t="n">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B62" s="0" t="n">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="B63" s="0" t="n">
-        <v>203</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="B64" s="0" t="n">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>336</v>
-      </c>
-      <c r="B65" s="0" t="n">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
-        <v>337</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
-        <v>339</v>
-      </c>
-      <c r="B70" s="0" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>341</v>
-      </c>
-      <c r="B71" s="0" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="B72" s="0" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="B73" s="0" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="0" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="B75" s="0" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="B76" s="0" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B77" s="0" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="B79" s="0" t="s">
-        <v>350</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -5617,25 +5598,594 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A9:C10"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>328</v>
+      </c>
+    </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B9" s="0" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="C9" s="0" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
         <v>353</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>181</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>182</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>149</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>183</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>184</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>185</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>186</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>153</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>187</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>188</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>155</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>189</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>157</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>191</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>158</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>192</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>193</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>160</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>203</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="0" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -5654,328 +6204,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A9:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>360</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>206</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>162</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>207</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>363</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>163</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>365</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>208</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>366</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>209</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>210</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>368</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>166</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <v>211</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>370</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>371</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <v>212</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="B20" s="0" t="n">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>373</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <v>214</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>216</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>376</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>217</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <v>218</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>379</v>
-      </c>
-      <c r="B27" s="0" t="n">
-        <v>220</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>381</v>
-      </c>
-      <c r="B28" s="0" t="n">
-        <v>221</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <v>222</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>384</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>223</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="0" t="n">
-        <v>224</v>
-      </c>
-      <c r="C31" s="0" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="C9" s="0" t="s">
         <v>387</v>
       </c>
-      <c r="B32" s="0" t="n">
-        <v>225</v>
-      </c>
-      <c r="C32" s="0" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>388</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -6000,7 +6247,7 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.1"/>
   </cols>

</xml_diff>